<commit_message>
Fake json data for analytics
</commit_message>
<xml_diff>
--- a/Documentation/Projects/Analytics/fakedata/data/datacollectors-2018-September-28 (1).xlsx
+++ b/Documentation/Projects/Analytics/fakedata/data/datacollectors-2018-September-28 (1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="110">
   <si>
     <t xml:space="preserve">Full Name</t>
   </si>
@@ -73,289 +73,280 @@
     <t xml:space="preserve">8.91819803872482, 57.2053597765304</t>
   </si>
   <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akershus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandefjord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aninek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.20061385863315, 49.2493295069055</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oslo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandeid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hodo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rebecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.6023317964317, 5.79999417056536</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ølen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48.3104189867626, 5.5852160999026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belingo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OleK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-8.45938540886102, -54.1538728584696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guddu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.60128193440505, 44.6859294804688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.22193720644296, 46.0152751835938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.5739103196699, 58.1470234999508</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wiik Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karoline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1694982828087, 44.05146903125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aust-Agder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anahi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.42791888704628, 44.7957927617188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SergeyS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.27073330982181, 45.5099040898438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaja Goplen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bamkao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Are4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.63702708140697, 44.8996135289724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cameroon street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peter Potsepp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.09200806228194, 12.6558280280044</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arif Shafiqje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.33578422443075, 46.1086589726563</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xavier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buskerud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOOD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kai Erland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.11890109199149, 46.4986736210938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thelin Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kemal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.95072581550045, 46.9546062382813</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hassan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finnmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alex Klein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.3799132668328, 71.8227529640193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Espen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.54711543675425, 44.0426799352224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.0692020863618, 68.1059751458157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karl Trollsaas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.59586567360916, 45.611527625</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thomas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.80162230069309, 47.2292644414063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hordaland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wedler Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">andrei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.14746220264844, 46.259720984375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ronny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.55253247492412, 44.1085979039724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nordland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FarrukhW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hedda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.70417438004702, 44.0459758671875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oppland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.56878307212513, 44.1085979039724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.52002895475, 44.1415568883474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mihaela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.51461140044883, 44.0646525914724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rogaland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Village20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tore Eggen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.7738199584651, 9.91060092201121</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vestfold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akershus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandefjord</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aninek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.20061385863315, 49.2493295069055</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Norway</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oslo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indian Ocean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hodo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rogaland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sandeid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rebecca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59.6023317964317, 5.79999417056536</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ølen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48.3104189867626, 5.5852160999026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Son</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OleK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-8.45938540886102, -54.1538728584696</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belingo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guddu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.60128193440505, 44.6859294804688</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.22193720644296, 46.0152751835938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">odwine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.5739103196699, 58.1470234999508</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lasondra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unknown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karoline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.1694982828087, 44.05146903125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aust-Agder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anahi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.42791888704628, 44.7957927617188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moroni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wiik Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SergeyS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.27073330982181, 45.5099040898438</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaja Goplen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bamkao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Are4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.63702708140697, 44.8996135289724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peter Potsepp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.09200806228194, 12.6558280280044</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Layuna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cameroon street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arif Shafiqje</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.33578422443075, 46.1086589726563</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xavier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XOOD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buskerud</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kai Erland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.11890109199149, 46.4986736210938</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thelin Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kemal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.95072581550045, 46.9546062382813</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hassan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finnmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alex Klein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.3799132668328, 71.8227529640193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Espen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.54711543675425, 44.0426799352224</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bahal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.0692020863618, 68.1059751458157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karl Trollsaas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.59586567360916, 45.611527625</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thomas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.80162230069309, 47.2292644414063</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hordaland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wedler Village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">andrei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.14746220264844, 46.259720984375</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ronny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.55253247492412, 44.1085979039724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nordland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FarrukhW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somewhere</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hedda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.70417438004702, 44.0459758671875</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oppland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ellen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.56878307212513, 44.1085979039724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">John Martin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.52002895475, 44.1415568883474</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mihaela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.51461140044883, 44.0646525914724</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tore Eggen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59.7738199584651, 9.91060092201121</t>
   </si>
   <si>
     <t xml:space="preserve">Hokksund</t>
@@ -445,12 +436,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -460,10 +451,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -561,13 +552,13 @@
         <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>12</v>
@@ -578,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1990</v>
@@ -593,13 +584,13 @@
         <v>16</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>12</v>
@@ -610,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1990</v>
@@ -625,13 +616,13 @@
         <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="J5" s="0" t="s">
         <v>12</v>
@@ -642,7 +633,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1990</v>
@@ -654,16 +645,16 @@
         <v>15</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J6" s="0" t="s">
         <v>12</v>
@@ -674,7 +665,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1990</v>
@@ -686,16 +677,16 @@
         <v>15</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J7" s="0" t="s">
         <v>12</v>
@@ -706,7 +697,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1990</v>
@@ -718,16 +709,16 @@
         <v>15</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="J8" s="0" t="s">
         <v>12</v>
@@ -738,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1990</v>
@@ -750,16 +741,16 @@
         <v>15</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>12</v>
@@ -770,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1990</v>
@@ -782,16 +773,16 @@
         <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J10" s="0" t="s">
         <v>12</v>
@@ -802,7 +793,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1990</v>
@@ -814,16 +805,16 @@
         <v>15</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>12</v>
@@ -834,7 +825,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1990</v>
@@ -846,16 +837,16 @@
         <v>15</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>12</v>
@@ -866,7 +857,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>1990</v>
@@ -878,16 +869,16 @@
         <v>15</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="J13" s="0" t="s">
         <v>12</v>
@@ -898,7 +889,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>1990</v>
@@ -910,16 +901,16 @@
         <v>15</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>12</v>
@@ -930,7 +921,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>1990</v>
@@ -942,16 +933,16 @@
         <v>15</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J15" s="0" t="s">
         <v>12</v>
@@ -962,7 +953,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>1990</v>
@@ -974,16 +965,16 @@
         <v>15</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J16" s="0" t="s">
         <v>12</v>
@@ -994,7 +985,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>1990</v>
@@ -1006,16 +997,16 @@
         <v>15</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J17" s="0" t="s">
         <v>12</v>
@@ -1026,7 +1017,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>1990</v>
@@ -1038,16 +1029,16 @@
         <v>15</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>12</v>
@@ -1058,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1990</v>
@@ -1070,16 +1061,16 @@
         <v>15</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="J19" s="0" t="s">
         <v>12</v>
@@ -1090,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1990</v>
@@ -1102,16 +1093,16 @@
         <v>15</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>12</v>
@@ -1122,7 +1113,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>1990</v>
@@ -1134,16 +1125,16 @@
         <v>15</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J21" s="0" t="s">
         <v>12</v>
@@ -1154,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1990</v>
@@ -1166,16 +1157,16 @@
         <v>15</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J22" s="0" t="s">
         <v>12</v>
@@ -1186,7 +1177,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>1990</v>
@@ -1198,16 +1189,16 @@
         <v>15</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>12</v>
@@ -1218,7 +1209,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>1990</v>
@@ -1230,16 +1221,16 @@
         <v>15</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="J24" s="0" t="s">
         <v>12</v>
@@ -1250,7 +1241,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>1990</v>
@@ -1262,16 +1253,16 @@
         <v>15</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>12</v>
@@ -1282,7 +1273,7 @@
         <v>12</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1990</v>
@@ -1294,16 +1285,16 @@
         <v>15</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J26" s="0" t="s">
         <v>12</v>
@@ -1314,7 +1305,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1990</v>
@@ -1326,16 +1317,16 @@
         <v>15</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="J27" s="0" t="s">
         <v>12</v>
@@ -1346,7 +1337,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>1990</v>
@@ -1358,16 +1349,16 @@
         <v>15</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J28" s="0" t="s">
         <v>12</v>
@@ -1378,7 +1369,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>1990</v>
@@ -1390,16 +1381,16 @@
         <v>15</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="J29" s="0" t="s">
         <v>12</v>
@@ -1410,7 +1401,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>1990</v>
@@ -1422,16 +1413,16 @@
         <v>15</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="J30" s="0" t="s">
         <v>12</v>
@@ -1442,7 +1433,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>1990</v>
@@ -1454,16 +1445,16 @@
         <v>15</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J31" s="0" t="s">
         <v>12</v>
@@ -1474,7 +1465,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>1990</v>
@@ -1486,16 +1477,16 @@
         <v>15</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="J32" s="0" t="s">
         <v>12</v>
@@ -1506,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>1990</v>
@@ -1518,16 +1509,16 @@
         <v>15</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
       <c r="J33" s="0" t="s">
         <v>12</v>
@@ -1538,7 +1529,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>1990</v>
@@ -1550,16 +1541,16 @@
         <v>15</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="J34" s="0" t="s">
         <v>12</v>
@@ -1570,7 +1561,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>1990</v>
@@ -1582,16 +1573,16 @@
         <v>15</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>12</v>

</xml_diff>